<commit_message>
Code to create study sample
</commit_message>
<xml_diff>
--- a/results/sample.xlsx
+++ b/results/sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="1024">
   <si>
     <t xml:space="preserve">Authors</t>
   </si>
@@ -2697,6 +2697,393 @@
   </si>
   <si>
     <t xml:space="preserve">2-s2.0-85067572556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glenn, C.R., Kleiman, E.M., Coppersmith, D.D.L., Santee, A.C., Esposito, E.C., Cha, C.B., Nock, M.K., Auerbach, R.P.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57200267735; 37031224700; 57194571341; 57191590964; 56742825800; 24175717900; 6701414081; 8696294300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implicit identification with death predicts change in suicide ideation during psychiatric treatment in adolescents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1111/jcpp.12769</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85021822040&amp;partnerID=40&amp;md5=13d17ba644fb331d794f0840c1d648cf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85021822040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montoya, A.K.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57191490526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderation analysis in two-instance repeated measures designs: Probing methods and multiple moderator models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.3758/s13428-018-1088-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85055119490&amp;partnerID=40&amp;md5=53b8a13fa1abe5948b5dd94b02c864a5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85055119490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ledgerwood, A., Eastwick, P.W., Smith, L.K.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57207509081; 15131266800; 57191224917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toward an Integrative Framework for Studying Human Evaluation: Attitudes Toward Objects and Attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personality and Social Psychology Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">398</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1177/1088868318790718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85053428602&amp;partnerID=40&amp;md5=fd8a8ed454813c6e933fb1661bbe440e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85053428602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10888683, 15327957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1997-ongoing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wang, C., Xu, G., Zhang, X.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15924354400; 55360765300; 57207920819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction for Item Response Theory Latent Trait Measurement Error in Linear Mixed Effects Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1007/s11336-019-09672-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85067309784&amp;partnerID=40&amp;md5=281ad92defd95b593d01e6749c8462fa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85067309784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schröder, J., Berger, T., Meyer, B., Lutz, W., Späth, C., Michel, P., Rose, M., Hautzinger, M., Hohagen, F., Klein, J.P., Moritz, S.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55253986100; 55169251100; 7402073273; 7202713172; 55908010200; 57200880678; 57203322368; 55865190800; 7004331252; 36758688900; 7005488974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impact and change of attitudes toward Internet interventions within a randomized controlled trial on individuals with depression symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depression and Anxiety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1002/da.22727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85042565759&amp;partnerID=40&amp;md5=37dc431d01cf82baac1a917a9ff91559</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85042565759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10914269, 15206394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hallgren, M., Skott, M., Ekblom, O., Firth, J., Schembri, A., Forsell, Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35072791900; 57201900217; 6603154125; 56503241000; 56669659800; 7003829458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise effects on cognitive functioning in young adults with first-episode psychosis: FitForLife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1017/S0033291718001022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85046479144&amp;partnerID=40&amp;md5=c2ad9114728abb5a07a6de4d02800c65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85046479144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ward, T., Garety, P.A., Jackson, M., Peters, E.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55534106600; 7004167371; 41661668200; 57210754039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinical and theoretical relevance of responses to analogues of psychotic experiences in people with psychotic experiences with and without a need-for-care: An experimental study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1017/S0033291719000576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85063891041&amp;partnerID=40&amp;md5=8c14e377d817625ccbc895dbdded5eaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85063891041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doré, B.P., Morris, R.R., Burr, D.A., Picard, R.W., Ochsner, K.N.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56592148300; 36492103600; 57192708015; 7005583409; 6603738607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helping Others Regulate Emotion Predicts Increased Regulation of One’s Own Emotions and Decreased Symptoms of Depression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">739</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1177/0146167217695558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85018993506&amp;partnerID=40&amp;md5=b0ec1a777690a622d54be7bef62ae18e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85018993506</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mair, P., Wilcox, R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16425720400; 7202527113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robust statistical methods in R using the WRS2 package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.3758/s13428-019-01246-w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85066619265&amp;partnerID=40&amp;md5=3861cb4c1d98d9fecba05e0e66ca6350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85066619265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black, C.N., Bot, M., Scheffer, P.G., Penninx, B.W.J.H.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56471261900; 35106795000; 7007049287; 55800249300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxidative stress in major depressive and anxiety disorders, and the association with antidepressant use; Results from a large adult cohort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">948</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1017/S0033291716002828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85001560586&amp;partnerID=40&amp;md5=cde786a0aced8350693c0f213754a4e2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85001560586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindriks, P., Verkuyten, M., Coenders, M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56058236100; 7006059165; 6508152143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluating Political Acculturation Strategies: The Perspective of the Majority and Other Minority Groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Political Psychology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1111/pops.12356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-84994613652&amp;partnerID=40&amp;md5=4b1fd33b40d45f2204838dd28f5b577a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-84994613652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0162895X, 14679221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinical Psychology (Q1); Experimental and Cognitive Psychology (Q1); Philosophy (Q1); Political Science and International Relations (Q1); Social Psychology (Q1); Sociology and Political Science (Q1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosenblau, G., O'Connell, G., Heekeren, H.R., Dziobek, I.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55391049800; 36657393800; 6602477996; 14023902800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neurobiological mechanisms of social cognition treatment in high-functioning adults with autism spectrum disorder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1017/S0033291719002472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85072649656&amp;partnerID=40&amp;md5=2de47270869fe31a6f4068f825cbd122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85072649656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outhwaite, L.A., Faulder, M., Gulliford, A., Pitchford, N.J.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57189713108; 57202677118; 41561210600; 6601967054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raising early achievement in math with interactive apps: A randomized control trial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal of Educational Psychology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1037/edu0000286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85049055184&amp;partnerID=40&amp;md5=2a97a8957f07ccd55c96c83848339f94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85049055184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00220663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1910-ongoing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barnicot, K., Crawford, M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57208633654; 57203219698</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclusions and questions from a non-randomised comparison of routine clinical services implementing different treatment models for borderline personality disorder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1017/S0033291719002447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85072647129&amp;partnerID=40&amp;md5=a1f175fe0656566208a43cc458cda751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85072647129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ball, C.L., Smetana, J.G., Sturge-Apple, M.L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55794696800; 35578722300; 8262592700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Following my head and my heart: Integrating preschoolers’ empathy, theory of mind, and moral judgments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">611</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1111/cdev.12605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-84992013297&amp;partnerID=40&amp;md5=2dfb73ff1b6433377a7fc5472f48e966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-84992013297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vize, C.E., Collison, K.L., Miller, J.D., Lynam, D.R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57191498479; 56426004000; 55547139304; 55416190700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examining the Effects of Controlling for Shared Variance among the Dark Triad Using Meta-analytic Structural Equation Modelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1002/per.2137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scopus.com/inward/record.url?eid=2-s2.0-85041008537&amp;partnerID=40&amp;md5=a52c8a16d07da244a7bd4b5146456388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-s2.0-85041008537</t>
   </si>
 </sst>
 </file>
@@ -12957,6 +13344,1966 @@
         <v>695</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>895</v>
+      </c>
+      <c r="B82" t="s">
+        <v>896</v>
+      </c>
+      <c r="C82" t="s">
+        <v>897</v>
+      </c>
+      <c r="D82" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E82" t="s">
+        <v>722</v>
+      </c>
+      <c r="F82" t="s">
+        <v>723</v>
+      </c>
+      <c r="G82" t="s">
+        <v>46</v>
+      </c>
+      <c r="H82" t="s">
+        <v>48</v>
+      </c>
+      <c r="I82" t="s">
+        <v>898</v>
+      </c>
+      <c r="J82" t="s">
+        <v>899</v>
+      </c>
+      <c r="K82"/>
+      <c r="L82" t="n">
+        <v>9</v>
+      </c>
+      <c r="M82" t="s">
+        <v>900</v>
+      </c>
+      <c r="N82" t="s">
+        <v>901</v>
+      </c>
+      <c r="O82" t="s">
+        <v>51</v>
+      </c>
+      <c r="P82" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>48</v>
+      </c>
+      <c r="R82" t="s">
+        <v>54</v>
+      </c>
+      <c r="S82" t="s">
+        <v>902</v>
+      </c>
+      <c r="T82" t="n">
+        <v>3946</v>
+      </c>
+      <c r="U82" t="n">
+        <v>31</v>
+      </c>
+      <c r="V82" t="n">
+        <v>15402</v>
+      </c>
+      <c r="W82" t="s">
+        <v>722</v>
+      </c>
+      <c r="X82" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>729</v>
+      </c>
+      <c r="Z82" t="n">
+        <v>3.305</v>
+      </c>
+      <c r="AA82" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB82" t="n">
+        <v>187</v>
+      </c>
+      <c r="AC82" t="n">
+        <v>167</v>
+      </c>
+      <c r="AD82" t="n">
+        <v>474</v>
+      </c>
+      <c r="AE82" t="n">
+        <v>7901</v>
+      </c>
+      <c r="AF82" t="n">
+        <v>2767</v>
+      </c>
+      <c r="AG82" t="n">
+        <v>391</v>
+      </c>
+      <c r="AH82" t="n">
+        <v>6.33</v>
+      </c>
+      <c r="AI82" t="n">
+        <v>47.31</v>
+      </c>
+      <c r="AJ82" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK82" t="s">
+        <v>730</v>
+      </c>
+      <c r="AL82" t="s">
+        <v>731</v>
+      </c>
+      <c r="AM82" t="s">
+        <v>732</v>
+      </c>
+      <c r="AN82" t="n">
+        <v>0.975020815986678</v>
+      </c>
+      <c r="AO82" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>903</v>
+      </c>
+      <c r="B83" t="s">
+        <v>904</v>
+      </c>
+      <c r="C83" t="s">
+        <v>905</v>
+      </c>
+      <c r="D83" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E83" t="s">
+        <v>748</v>
+      </c>
+      <c r="F83" t="s">
+        <v>810</v>
+      </c>
+      <c r="G83" t="s">
+        <v>165</v>
+      </c>
+      <c r="H83" t="s">
+        <v>48</v>
+      </c>
+      <c r="I83" t="s">
+        <v>776</v>
+      </c>
+      <c r="J83" t="s">
+        <v>797</v>
+      </c>
+      <c r="K83"/>
+      <c r="L83" t="n">
+        <v>4</v>
+      </c>
+      <c r="M83" t="s">
+        <v>906</v>
+      </c>
+      <c r="N83" t="s">
+        <v>907</v>
+      </c>
+      <c r="O83" t="s">
+        <v>51</v>
+      </c>
+      <c r="P83" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>48</v>
+      </c>
+      <c r="R83" t="s">
+        <v>54</v>
+      </c>
+      <c r="S83" t="s">
+        <v>908</v>
+      </c>
+      <c r="T83" t="n">
+        <v>1067</v>
+      </c>
+      <c r="U83" t="n">
+        <v>55</v>
+      </c>
+      <c r="V83" t="n">
+        <v>146223</v>
+      </c>
+      <c r="W83" t="s">
+        <v>748</v>
+      </c>
+      <c r="X83" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>755</v>
+      </c>
+      <c r="Z83" t="n">
+        <v>2.686</v>
+      </c>
+      <c r="AA83" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB83" t="n">
+        <v>114</v>
+      </c>
+      <c r="AC83" t="n">
+        <v>273</v>
+      </c>
+      <c r="AD83" t="n">
+        <v>390</v>
+      </c>
+      <c r="AE83" t="n">
+        <v>13654</v>
+      </c>
+      <c r="AF83" t="n">
+        <v>1689</v>
+      </c>
+      <c r="AG83" t="n">
+        <v>373</v>
+      </c>
+      <c r="AH83" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="AI83" t="n">
+        <v>50.01</v>
+      </c>
+      <c r="AJ83" t="s">
+        <v>756</v>
+      </c>
+      <c r="AK83" t="s">
+        <v>757</v>
+      </c>
+      <c r="AL83" t="s">
+        <v>758</v>
+      </c>
+      <c r="AM83" t="s">
+        <v>759</v>
+      </c>
+      <c r="AN83" t="n">
+        <v>0.95503746877602</v>
+      </c>
+      <c r="AO83" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>909</v>
+      </c>
+      <c r="B84" t="s">
+        <v>910</v>
+      </c>
+      <c r="C84" t="s">
+        <v>911</v>
+      </c>
+      <c r="D84" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E84" t="s">
+        <v>912</v>
+      </c>
+      <c r="F84" t="s">
+        <v>658</v>
+      </c>
+      <c r="G84" t="s">
+        <v>233</v>
+      </c>
+      <c r="H84" t="s">
+        <v>48</v>
+      </c>
+      <c r="I84" t="s">
+        <v>913</v>
+      </c>
+      <c r="J84" t="s">
+        <v>914</v>
+      </c>
+      <c r="K84"/>
+      <c r="L84" t="n">
+        <v>3</v>
+      </c>
+      <c r="M84" t="s">
+        <v>915</v>
+      </c>
+      <c r="N84" t="s">
+        <v>916</v>
+      </c>
+      <c r="O84" t="s">
+        <v>51</v>
+      </c>
+      <c r="P84" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>48</v>
+      </c>
+      <c r="R84" t="s">
+        <v>54</v>
+      </c>
+      <c r="S84" t="s">
+        <v>917</v>
+      </c>
+      <c r="T84" t="n">
+        <v>2142</v>
+      </c>
+      <c r="U84" t="n">
+        <v>3</v>
+      </c>
+      <c r="V84" t="n">
+        <v>12812</v>
+      </c>
+      <c r="W84" t="s">
+        <v>912</v>
+      </c>
+      <c r="X84" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>918</v>
+      </c>
+      <c r="Z84" t="n">
+        <v>7.807</v>
+      </c>
+      <c r="AA84" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB84" t="n">
+        <v>134</v>
+      </c>
+      <c r="AC84" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD84" t="n">
+        <v>49</v>
+      </c>
+      <c r="AE84" t="n">
+        <v>3264</v>
+      </c>
+      <c r="AF84" t="n">
+        <v>639</v>
+      </c>
+      <c r="AG84" t="n">
+        <v>48</v>
+      </c>
+      <c r="AH84" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="AI84" t="n">
+        <v>130.56</v>
+      </c>
+      <c r="AJ84" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK84" t="s">
+        <v>254</v>
+      </c>
+      <c r="AL84" t="s">
+        <v>919</v>
+      </c>
+      <c r="AM84" t="s">
+        <v>707</v>
+      </c>
+      <c r="AN84" t="n">
+        <v>0.998334721065778</v>
+      </c>
+      <c r="AO84" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>920</v>
+      </c>
+      <c r="B85" t="s">
+        <v>921</v>
+      </c>
+      <c r="C85" t="s">
+        <v>922</v>
+      </c>
+      <c r="D85" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E85" t="s">
+        <v>796</v>
+      </c>
+      <c r="F85" t="s">
+        <v>883</v>
+      </c>
+      <c r="G85" t="s">
+        <v>68</v>
+      </c>
+      <c r="H85" t="s">
+        <v>48</v>
+      </c>
+      <c r="I85" t="s">
+        <v>923</v>
+      </c>
+      <c r="J85" t="s">
+        <v>924</v>
+      </c>
+      <c r="K85"/>
+      <c r="L85"/>
+      <c r="M85" t="s">
+        <v>925</v>
+      </c>
+      <c r="N85" t="s">
+        <v>926</v>
+      </c>
+      <c r="O85" t="s">
+        <v>51</v>
+      </c>
+      <c r="P85" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>48</v>
+      </c>
+      <c r="R85" t="s">
+        <v>54</v>
+      </c>
+      <c r="S85" t="s">
+        <v>927</v>
+      </c>
+      <c r="T85" t="n">
+        <v>220</v>
+      </c>
+      <c r="U85" t="n">
+        <v>42</v>
+      </c>
+      <c r="V85" t="n">
+        <v>14061</v>
+      </c>
+      <c r="W85" t="s">
+        <v>796</v>
+      </c>
+      <c r="X85" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>803</v>
+      </c>
+      <c r="Z85" t="n">
+        <v>3.012</v>
+      </c>
+      <c r="AA85" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB85" t="n">
+        <v>68</v>
+      </c>
+      <c r="AC85" t="n">
+        <v>56</v>
+      </c>
+      <c r="AD85" t="n">
+        <v>176</v>
+      </c>
+      <c r="AE85" t="n">
+        <v>2140</v>
+      </c>
+      <c r="AF85" t="n">
+        <v>466</v>
+      </c>
+      <c r="AG85" t="n">
+        <v>165</v>
+      </c>
+      <c r="AH85" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="AI85" t="n">
+        <v>38.21</v>
+      </c>
+      <c r="AJ85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK85" t="s">
+        <v>804</v>
+      </c>
+      <c r="AL85" t="s">
+        <v>805</v>
+      </c>
+      <c r="AM85" t="s">
+        <v>806</v>
+      </c>
+      <c r="AN85" t="n">
+        <v>0.96586178184846</v>
+      </c>
+      <c r="AO85" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>928</v>
+      </c>
+      <c r="B86" t="s">
+        <v>929</v>
+      </c>
+      <c r="C86" t="s">
+        <v>930</v>
+      </c>
+      <c r="D86" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E86" t="s">
+        <v>931</v>
+      </c>
+      <c r="F86" t="s">
+        <v>97</v>
+      </c>
+      <c r="G86" t="s">
+        <v>142</v>
+      </c>
+      <c r="H86" t="s">
+        <v>48</v>
+      </c>
+      <c r="I86" t="s">
+        <v>932</v>
+      </c>
+      <c r="J86" t="s">
+        <v>933</v>
+      </c>
+      <c r="K86"/>
+      <c r="L86" t="n">
+        <v>2</v>
+      </c>
+      <c r="M86" t="s">
+        <v>934</v>
+      </c>
+      <c r="N86" t="s">
+        <v>935</v>
+      </c>
+      <c r="O86" t="s">
+        <v>51</v>
+      </c>
+      <c r="P86" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>48</v>
+      </c>
+      <c r="R86" t="s">
+        <v>54</v>
+      </c>
+      <c r="S86" t="s">
+        <v>936</v>
+      </c>
+      <c r="T86" t="n">
+        <v>2977</v>
+      </c>
+      <c r="U86" t="n">
+        <v>47</v>
+      </c>
+      <c r="V86" t="n">
+        <v>13487</v>
+      </c>
+      <c r="W86" t="s">
+        <v>931</v>
+      </c>
+      <c r="X86" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>937</v>
+      </c>
+      <c r="Z86" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB86" t="n">
+        <v>110</v>
+      </c>
+      <c r="AC86" t="n">
+        <v>129</v>
+      </c>
+      <c r="AD86" t="n">
+        <v>354</v>
+      </c>
+      <c r="AE86" t="n">
+        <v>6350</v>
+      </c>
+      <c r="AF86" t="n">
+        <v>1883</v>
+      </c>
+      <c r="AG86" t="n">
+        <v>315</v>
+      </c>
+      <c r="AH86" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="AI86" t="n">
+        <v>49.22</v>
+      </c>
+      <c r="AJ86" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK86" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL86" t="s">
+        <v>665</v>
+      </c>
+      <c r="AM86" t="s">
+        <v>850</v>
+      </c>
+      <c r="AN86" t="n">
+        <v>0.961698584512906</v>
+      </c>
+      <c r="AO86" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>938</v>
+      </c>
+      <c r="B87" t="s">
+        <v>939</v>
+      </c>
+      <c r="C87" t="s">
+        <v>940</v>
+      </c>
+      <c r="D87" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E87" t="s">
+        <v>763</v>
+      </c>
+      <c r="F87" t="s">
+        <v>574</v>
+      </c>
+      <c r="G87" t="s">
+        <v>68</v>
+      </c>
+      <c r="H87" t="s">
+        <v>48</v>
+      </c>
+      <c r="I87" t="s">
+        <v>941</v>
+      </c>
+      <c r="J87" t="s">
+        <v>942</v>
+      </c>
+      <c r="K87"/>
+      <c r="L87" t="n">
+        <v>2</v>
+      </c>
+      <c r="M87" t="s">
+        <v>943</v>
+      </c>
+      <c r="N87" t="s">
+        <v>944</v>
+      </c>
+      <c r="O87" t="s">
+        <v>51</v>
+      </c>
+      <c r="P87" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>48</v>
+      </c>
+      <c r="R87" t="s">
+        <v>54</v>
+      </c>
+      <c r="S87" t="s">
+        <v>945</v>
+      </c>
+      <c r="T87" t="n">
+        <v>1185</v>
+      </c>
+      <c r="U87" t="n">
+        <v>39</v>
+      </c>
+      <c r="V87" t="n">
+        <v>18742</v>
+      </c>
+      <c r="W87" t="s">
+        <v>763</v>
+      </c>
+      <c r="X87" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>770</v>
+      </c>
+      <c r="Z87" t="n">
+        <v>3.077</v>
+      </c>
+      <c r="AA87" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB87" t="n">
+        <v>188</v>
+      </c>
+      <c r="AC87" t="n">
+        <v>430</v>
+      </c>
+      <c r="AD87" t="n">
+        <v>869</v>
+      </c>
+      <c r="AE87" t="n">
+        <v>19438</v>
+      </c>
+      <c r="AF87" t="n">
+        <v>5020</v>
+      </c>
+      <c r="AG87" t="n">
+        <v>809</v>
+      </c>
+      <c r="AH87" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AI87" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="AJ87" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK87" t="s">
+        <v>771</v>
+      </c>
+      <c r="AL87" t="s">
+        <v>518</v>
+      </c>
+      <c r="AM87" t="s">
+        <v>772</v>
+      </c>
+      <c r="AN87" t="n">
+        <v>0.968359700249792</v>
+      </c>
+      <c r="AO87" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>946</v>
+      </c>
+      <c r="B88" t="s">
+        <v>947</v>
+      </c>
+      <c r="C88" t="s">
+        <v>948</v>
+      </c>
+      <c r="D88" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E88" t="s">
+        <v>763</v>
+      </c>
+      <c r="F88" t="s">
+        <v>48</v>
+      </c>
+      <c r="G88" t="s">
+        <v>48</v>
+      </c>
+      <c r="H88" t="s">
+        <v>48</v>
+      </c>
+      <c r="I88" t="s">
+        <v>48</v>
+      </c>
+      <c r="J88" t="s">
+        <v>48</v>
+      </c>
+      <c r="K88"/>
+      <c r="L88"/>
+      <c r="M88" t="s">
+        <v>949</v>
+      </c>
+      <c r="N88" t="s">
+        <v>950</v>
+      </c>
+      <c r="O88" t="s">
+        <v>51</v>
+      </c>
+      <c r="P88" t="s">
+        <v>833</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>48</v>
+      </c>
+      <c r="R88" t="s">
+        <v>54</v>
+      </c>
+      <c r="S88" t="s">
+        <v>951</v>
+      </c>
+      <c r="T88" t="n">
+        <v>1797</v>
+      </c>
+      <c r="U88" t="n">
+        <v>39</v>
+      </c>
+      <c r="V88" t="n">
+        <v>18742</v>
+      </c>
+      <c r="W88" t="s">
+        <v>763</v>
+      </c>
+      <c r="X88" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y88" t="s">
+        <v>770</v>
+      </c>
+      <c r="Z88" t="n">
+        <v>3.077</v>
+      </c>
+      <c r="AA88" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB88" t="n">
+        <v>188</v>
+      </c>
+      <c r="AC88" t="n">
+        <v>430</v>
+      </c>
+      <c r="AD88" t="n">
+        <v>869</v>
+      </c>
+      <c r="AE88" t="n">
+        <v>19438</v>
+      </c>
+      <c r="AF88" t="n">
+        <v>5020</v>
+      </c>
+      <c r="AG88" t="n">
+        <v>809</v>
+      </c>
+      <c r="AH88" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AI88" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="AJ88" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK88" t="s">
+        <v>771</v>
+      </c>
+      <c r="AL88" t="s">
+        <v>518</v>
+      </c>
+      <c r="AM88" t="s">
+        <v>772</v>
+      </c>
+      <c r="AN88" t="n">
+        <v>0.968359700249792</v>
+      </c>
+      <c r="AO88" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>952</v>
+      </c>
+      <c r="B89" t="s">
+        <v>953</v>
+      </c>
+      <c r="C89" t="s">
+        <v>954</v>
+      </c>
+      <c r="D89" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E89" t="s">
+        <v>819</v>
+      </c>
+      <c r="F89" t="s">
+        <v>955</v>
+      </c>
+      <c r="G89" t="s">
+        <v>142</v>
+      </c>
+      <c r="H89" t="s">
+        <v>48</v>
+      </c>
+      <c r="I89" t="s">
+        <v>956</v>
+      </c>
+      <c r="J89" t="s">
+        <v>957</v>
+      </c>
+      <c r="K89"/>
+      <c r="L89" t="n">
+        <v>11</v>
+      </c>
+      <c r="M89" t="s">
+        <v>958</v>
+      </c>
+      <c r="N89" t="s">
+        <v>959</v>
+      </c>
+      <c r="O89" t="s">
+        <v>51</v>
+      </c>
+      <c r="P89" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>48</v>
+      </c>
+      <c r="R89" t="s">
+        <v>54</v>
+      </c>
+      <c r="S89" t="s">
+        <v>960</v>
+      </c>
+      <c r="T89" t="n">
+        <v>4867</v>
+      </c>
+      <c r="U89" t="n">
+        <v>61</v>
+      </c>
+      <c r="V89" t="n">
+        <v>12811</v>
+      </c>
+      <c r="W89" t="s">
+        <v>819</v>
+      </c>
+      <c r="X89" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y89" t="s">
+        <v>825</v>
+      </c>
+      <c r="Z89" t="n">
+        <v>2.481</v>
+      </c>
+      <c r="AA89" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB89" t="n">
+        <v>172</v>
+      </c>
+      <c r="AC89" t="n">
+        <v>155</v>
+      </c>
+      <c r="AD89" t="n">
+        <v>363</v>
+      </c>
+      <c r="AE89" t="n">
+        <v>9084</v>
+      </c>
+      <c r="AF89" t="n">
+        <v>1357</v>
+      </c>
+      <c r="AG89" t="n">
+        <v>355</v>
+      </c>
+      <c r="AH89" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="AI89" t="n">
+        <v>58.61</v>
+      </c>
+      <c r="AJ89" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK89" t="s">
+        <v>254</v>
+      </c>
+      <c r="AL89" t="s">
+        <v>826</v>
+      </c>
+      <c r="AM89" t="s">
+        <v>707</v>
+      </c>
+      <c r="AN89" t="n">
+        <v>0.950041631973356</v>
+      </c>
+      <c r="AO89" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>961</v>
+      </c>
+      <c r="B90" t="s">
+        <v>962</v>
+      </c>
+      <c r="C90" t="s">
+        <v>963</v>
+      </c>
+      <c r="D90" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E90" t="s">
+        <v>748</v>
+      </c>
+      <c r="F90" t="s">
+        <v>48</v>
+      </c>
+      <c r="G90" t="s">
+        <v>48</v>
+      </c>
+      <c r="H90" t="s">
+        <v>48</v>
+      </c>
+      <c r="I90" t="s">
+        <v>48</v>
+      </c>
+      <c r="J90" t="s">
+        <v>48</v>
+      </c>
+      <c r="K90"/>
+      <c r="L90" t="n">
+        <v>3</v>
+      </c>
+      <c r="M90" t="s">
+        <v>964</v>
+      </c>
+      <c r="N90" t="s">
+        <v>965</v>
+      </c>
+      <c r="O90" t="s">
+        <v>51</v>
+      </c>
+      <c r="P90" t="s">
+        <v>833</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>48</v>
+      </c>
+      <c r="R90" t="s">
+        <v>54</v>
+      </c>
+      <c r="S90" t="s">
+        <v>966</v>
+      </c>
+      <c r="T90" t="n">
+        <v>1265</v>
+      </c>
+      <c r="U90" t="n">
+        <v>55</v>
+      </c>
+      <c r="V90" t="n">
+        <v>146223</v>
+      </c>
+      <c r="W90" t="s">
+        <v>748</v>
+      </c>
+      <c r="X90" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y90" t="s">
+        <v>755</v>
+      </c>
+      <c r="Z90" t="n">
+        <v>2.686</v>
+      </c>
+      <c r="AA90" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB90" t="n">
+        <v>114</v>
+      </c>
+      <c r="AC90" t="n">
+        <v>273</v>
+      </c>
+      <c r="AD90" t="n">
+        <v>390</v>
+      </c>
+      <c r="AE90" t="n">
+        <v>13654</v>
+      </c>
+      <c r="AF90" t="n">
+        <v>1689</v>
+      </c>
+      <c r="AG90" t="n">
+        <v>373</v>
+      </c>
+      <c r="AH90" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="AI90" t="n">
+        <v>50.01</v>
+      </c>
+      <c r="AJ90" t="s">
+        <v>756</v>
+      </c>
+      <c r="AK90" t="s">
+        <v>757</v>
+      </c>
+      <c r="AL90" t="s">
+        <v>758</v>
+      </c>
+      <c r="AM90" t="s">
+        <v>759</v>
+      </c>
+      <c r="AN90" t="n">
+        <v>0.95503746877602</v>
+      </c>
+      <c r="AO90" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>967</v>
+      </c>
+      <c r="B91" t="s">
+        <v>968</v>
+      </c>
+      <c r="C91" t="s">
+        <v>969</v>
+      </c>
+      <c r="D91" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E91" t="s">
+        <v>763</v>
+      </c>
+      <c r="F91" t="s">
+        <v>764</v>
+      </c>
+      <c r="G91" t="s">
+        <v>142</v>
+      </c>
+      <c r="H91" t="s">
+        <v>48</v>
+      </c>
+      <c r="I91" t="s">
+        <v>559</v>
+      </c>
+      <c r="J91" t="s">
+        <v>970</v>
+      </c>
+      <c r="K91"/>
+      <c r="L91" t="n">
+        <v>7</v>
+      </c>
+      <c r="M91" t="s">
+        <v>971</v>
+      </c>
+      <c r="N91" t="s">
+        <v>972</v>
+      </c>
+      <c r="O91" t="s">
+        <v>51</v>
+      </c>
+      <c r="P91" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>48</v>
+      </c>
+      <c r="R91" t="s">
+        <v>54</v>
+      </c>
+      <c r="S91" t="s">
+        <v>973</v>
+      </c>
+      <c r="T91" t="n">
+        <v>5065</v>
+      </c>
+      <c r="U91" t="n">
+        <v>39</v>
+      </c>
+      <c r="V91" t="n">
+        <v>18742</v>
+      </c>
+      <c r="W91" t="s">
+        <v>763</v>
+      </c>
+      <c r="X91" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>770</v>
+      </c>
+      <c r="Z91" t="n">
+        <v>3.077</v>
+      </c>
+      <c r="AA91" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB91" t="n">
+        <v>188</v>
+      </c>
+      <c r="AC91" t="n">
+        <v>430</v>
+      </c>
+      <c r="AD91" t="n">
+        <v>869</v>
+      </c>
+      <c r="AE91" t="n">
+        <v>19438</v>
+      </c>
+      <c r="AF91" t="n">
+        <v>5020</v>
+      </c>
+      <c r="AG91" t="n">
+        <v>809</v>
+      </c>
+      <c r="AH91" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AI91" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="AJ91" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK91" t="s">
+        <v>771</v>
+      </c>
+      <c r="AL91" t="s">
+        <v>518</v>
+      </c>
+      <c r="AM91" t="s">
+        <v>772</v>
+      </c>
+      <c r="AN91" t="n">
+        <v>0.968359700249792</v>
+      </c>
+      <c r="AO91" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>974</v>
+      </c>
+      <c r="B92" t="s">
+        <v>975</v>
+      </c>
+      <c r="C92" t="s">
+        <v>976</v>
+      </c>
+      <c r="D92" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E92" t="s">
+        <v>977</v>
+      </c>
+      <c r="F92" t="s">
+        <v>275</v>
+      </c>
+      <c r="G92" t="s">
+        <v>142</v>
+      </c>
+      <c r="H92" t="s">
+        <v>48</v>
+      </c>
+      <c r="I92" t="s">
+        <v>978</v>
+      </c>
+      <c r="J92" t="s">
+        <v>979</v>
+      </c>
+      <c r="K92"/>
+      <c r="L92" t="n">
+        <v>4</v>
+      </c>
+      <c r="M92" t="s">
+        <v>980</v>
+      </c>
+      <c r="N92" t="s">
+        <v>981</v>
+      </c>
+      <c r="O92" t="s">
+        <v>51</v>
+      </c>
+      <c r="P92" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>48</v>
+      </c>
+      <c r="R92" t="s">
+        <v>54</v>
+      </c>
+      <c r="S92" t="s">
+        <v>982</v>
+      </c>
+      <c r="T92" t="n">
+        <v>4220</v>
+      </c>
+      <c r="U92" t="n">
+        <v>38</v>
+      </c>
+      <c r="V92" t="n">
+        <v>22861</v>
+      </c>
+      <c r="W92" t="s">
+        <v>977</v>
+      </c>
+      <c r="X92" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y92" t="s">
+        <v>983</v>
+      </c>
+      <c r="Z92" t="n">
+        <v>3.094</v>
+      </c>
+      <c r="AA92" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB92" t="n">
+        <v>80</v>
+      </c>
+      <c r="AC92" t="n">
+        <v>123</v>
+      </c>
+      <c r="AD92" t="n">
+        <v>178</v>
+      </c>
+      <c r="AE92" t="n">
+        <v>7737</v>
+      </c>
+      <c r="AF92" t="n">
+        <v>812</v>
+      </c>
+      <c r="AG92" t="n">
+        <v>176</v>
+      </c>
+      <c r="AH92" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="AI92" t="n">
+        <v>62.9</v>
+      </c>
+      <c r="AJ92" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK92" t="s">
+        <v>730</v>
+      </c>
+      <c r="AL92" t="s">
+        <v>665</v>
+      </c>
+      <c r="AM92" t="s">
+        <v>984</v>
+      </c>
+      <c r="AN92" t="n">
+        <v>0.969192339716903</v>
+      </c>
+      <c r="AO92" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>985</v>
+      </c>
+      <c r="B93" t="s">
+        <v>986</v>
+      </c>
+      <c r="C93" t="s">
+        <v>987</v>
+      </c>
+      <c r="D93" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E93" t="s">
+        <v>763</v>
+      </c>
+      <c r="F93" t="s">
+        <v>48</v>
+      </c>
+      <c r="G93" t="s">
+        <v>48</v>
+      </c>
+      <c r="H93" t="s">
+        <v>48</v>
+      </c>
+      <c r="I93" t="s">
+        <v>48</v>
+      </c>
+      <c r="J93" t="s">
+        <v>48</v>
+      </c>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93" t="s">
+        <v>988</v>
+      </c>
+      <c r="N93" t="s">
+        <v>989</v>
+      </c>
+      <c r="O93" t="s">
+        <v>51</v>
+      </c>
+      <c r="P93" t="s">
+        <v>833</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>48</v>
+      </c>
+      <c r="R93" t="s">
+        <v>54</v>
+      </c>
+      <c r="S93" t="s">
+        <v>990</v>
+      </c>
+      <c r="T93" t="n">
+        <v>1827</v>
+      </c>
+      <c r="U93" t="n">
+        <v>39</v>
+      </c>
+      <c r="V93" t="n">
+        <v>18742</v>
+      </c>
+      <c r="W93" t="s">
+        <v>763</v>
+      </c>
+      <c r="X93" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y93" t="s">
+        <v>770</v>
+      </c>
+      <c r="Z93" t="n">
+        <v>3.077</v>
+      </c>
+      <c r="AA93" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB93" t="n">
+        <v>188</v>
+      </c>
+      <c r="AC93" t="n">
+        <v>430</v>
+      </c>
+      <c r="AD93" t="n">
+        <v>869</v>
+      </c>
+      <c r="AE93" t="n">
+        <v>19438</v>
+      </c>
+      <c r="AF93" t="n">
+        <v>5020</v>
+      </c>
+      <c r="AG93" t="n">
+        <v>809</v>
+      </c>
+      <c r="AH93" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AI93" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="AJ93" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK93" t="s">
+        <v>771</v>
+      </c>
+      <c r="AL93" t="s">
+        <v>518</v>
+      </c>
+      <c r="AM93" t="s">
+        <v>772</v>
+      </c>
+      <c r="AN93" t="n">
+        <v>0.968359700249792</v>
+      </c>
+      <c r="AO93" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>991</v>
+      </c>
+      <c r="B94" t="s">
+        <v>992</v>
+      </c>
+      <c r="C94" t="s">
+        <v>993</v>
+      </c>
+      <c r="D94" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E94" t="s">
+        <v>994</v>
+      </c>
+      <c r="F94" t="s">
+        <v>995</v>
+      </c>
+      <c r="G94" t="s">
+        <v>498</v>
+      </c>
+      <c r="H94" t="s">
+        <v>48</v>
+      </c>
+      <c r="I94" t="s">
+        <v>996</v>
+      </c>
+      <c r="J94" t="s">
+        <v>997</v>
+      </c>
+      <c r="K94"/>
+      <c r="L94" t="n">
+        <v>4</v>
+      </c>
+      <c r="M94" t="s">
+        <v>998</v>
+      </c>
+      <c r="N94" t="s">
+        <v>999</v>
+      </c>
+      <c r="O94" t="s">
+        <v>51</v>
+      </c>
+      <c r="P94" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>53</v>
+      </c>
+      <c r="R94" t="s">
+        <v>54</v>
+      </c>
+      <c r="S94" t="s">
+        <v>1000</v>
+      </c>
+      <c r="T94" t="n">
+        <v>1190</v>
+      </c>
+      <c r="U94" t="n">
+        <v>29</v>
+      </c>
+      <c r="V94" t="n">
+        <v>12808</v>
+      </c>
+      <c r="W94" t="s">
+        <v>994</v>
+      </c>
+      <c r="X94" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y94" t="s">
+        <v>1001</v>
+      </c>
+      <c r="Z94" t="n">
+        <v>3.459</v>
+      </c>
+      <c r="AA94" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB94" t="n">
+        <v>177</v>
+      </c>
+      <c r="AC94" t="n">
+        <v>113</v>
+      </c>
+      <c r="AD94" t="n">
+        <v>235</v>
+      </c>
+      <c r="AE94" t="n">
+        <v>6214</v>
+      </c>
+      <c r="AF94" t="n">
+        <v>1368</v>
+      </c>
+      <c r="AG94" t="n">
+        <v>222</v>
+      </c>
+      <c r="AH94" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="AI94" t="n">
+        <v>54.99</v>
+      </c>
+      <c r="AJ94" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK94" t="s">
+        <v>552</v>
+      </c>
+      <c r="AL94" t="s">
+        <v>1002</v>
+      </c>
+      <c r="AM94" t="s">
+        <v>718</v>
+      </c>
+      <c r="AN94" t="n">
+        <v>0.976686094920899</v>
+      </c>
+      <c r="AO94" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D95" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E95" t="s">
+        <v>763</v>
+      </c>
+      <c r="F95" t="s">
+        <v>48</v>
+      </c>
+      <c r="G95" t="s">
+        <v>48</v>
+      </c>
+      <c r="H95" t="s">
+        <v>48</v>
+      </c>
+      <c r="I95" t="s">
+        <v>48</v>
+      </c>
+      <c r="J95" t="s">
+        <v>48</v>
+      </c>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95" t="s">
+        <v>1006</v>
+      </c>
+      <c r="N95" t="s">
+        <v>1007</v>
+      </c>
+      <c r="O95" t="s">
+        <v>51</v>
+      </c>
+      <c r="P95" t="s">
+        <v>833</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>53</v>
+      </c>
+      <c r="R95" t="s">
+        <v>54</v>
+      </c>
+      <c r="S95" t="s">
+        <v>1008</v>
+      </c>
+      <c r="T95" t="n">
+        <v>1304</v>
+      </c>
+      <c r="U95" t="n">
+        <v>39</v>
+      </c>
+      <c r="V95" t="n">
+        <v>18742</v>
+      </c>
+      <c r="W95" t="s">
+        <v>763</v>
+      </c>
+      <c r="X95" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y95" t="s">
+        <v>770</v>
+      </c>
+      <c r="Z95" t="n">
+        <v>3.077</v>
+      </c>
+      <c r="AA95" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB95" t="n">
+        <v>188</v>
+      </c>
+      <c r="AC95" t="n">
+        <v>430</v>
+      </c>
+      <c r="AD95" t="n">
+        <v>869</v>
+      </c>
+      <c r="AE95" t="n">
+        <v>19438</v>
+      </c>
+      <c r="AF95" t="n">
+        <v>5020</v>
+      </c>
+      <c r="AG95" t="n">
+        <v>809</v>
+      </c>
+      <c r="AH95" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AI95" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="AJ95" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK95" t="s">
+        <v>771</v>
+      </c>
+      <c r="AL95" t="s">
+        <v>518</v>
+      </c>
+      <c r="AM95" t="s">
+        <v>772</v>
+      </c>
+      <c r="AN95" t="n">
+        <v>0.968359700249792</v>
+      </c>
+      <c r="AO95" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D96" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E96" t="s">
+        <v>783</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G96" t="s">
+        <v>498</v>
+      </c>
+      <c r="H96" t="s">
+        <v>48</v>
+      </c>
+      <c r="I96" t="s">
+        <v>1013</v>
+      </c>
+      <c r="J96" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K96"/>
+      <c r="L96" t="n">
+        <v>19</v>
+      </c>
+      <c r="M96" t="s">
+        <v>1015</v>
+      </c>
+      <c r="N96" t="s">
+        <v>1016</v>
+      </c>
+      <c r="O96" t="s">
+        <v>51</v>
+      </c>
+      <c r="P96" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>48</v>
+      </c>
+      <c r="R96" t="s">
+        <v>54</v>
+      </c>
+      <c r="S96" t="s">
+        <v>1017</v>
+      </c>
+      <c r="T96" t="n">
+        <v>5128</v>
+      </c>
+      <c r="U96" t="n">
+        <v>41</v>
+      </c>
+      <c r="V96" t="n">
+        <v>24456</v>
+      </c>
+      <c r="W96" t="s">
+        <v>783</v>
+      </c>
+      <c r="X96" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y96" t="s">
+        <v>790</v>
+      </c>
+      <c r="Z96" t="n">
+        <v>3.024</v>
+      </c>
+      <c r="AA96" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB96" t="n">
+        <v>228</v>
+      </c>
+      <c r="AC96" t="n">
+        <v>288</v>
+      </c>
+      <c r="AD96" t="n">
+        <v>477</v>
+      </c>
+      <c r="AE96" t="n">
+        <v>14343</v>
+      </c>
+      <c r="AF96" t="n">
+        <v>2412</v>
+      </c>
+      <c r="AG96" t="n">
+        <v>438</v>
+      </c>
+      <c r="AH96" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="AI96" t="n">
+        <v>49.8</v>
+      </c>
+      <c r="AJ96" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK96" t="s">
+        <v>730</v>
+      </c>
+      <c r="AL96" t="s">
+        <v>791</v>
+      </c>
+      <c r="AM96" t="s">
+        <v>792</v>
+      </c>
+      <c r="AN96" t="n">
+        <v>0.96669442131557</v>
+      </c>
+      <c r="AO96" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D97" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E97" t="s">
+        <v>699</v>
+      </c>
+      <c r="F97" t="s">
+        <v>154</v>
+      </c>
+      <c r="G97" t="s">
+        <v>165</v>
+      </c>
+      <c r="H97" t="s">
+        <v>48</v>
+      </c>
+      <c r="I97" t="s">
+        <v>276</v>
+      </c>
+      <c r="J97" t="s">
+        <v>776</v>
+      </c>
+      <c r="K97"/>
+      <c r="L97" t="n">
+        <v>15</v>
+      </c>
+      <c r="M97" t="s">
+        <v>1021</v>
+      </c>
+      <c r="N97" t="s">
+        <v>1022</v>
+      </c>
+      <c r="O97" t="s">
+        <v>51</v>
+      </c>
+      <c r="P97" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>48</v>
+      </c>
+      <c r="R97" t="s">
+        <v>54</v>
+      </c>
+      <c r="S97" t="s">
+        <v>1023</v>
+      </c>
+      <c r="T97" t="n">
+        <v>3762</v>
+      </c>
+      <c r="U97" t="n">
+        <v>57</v>
+      </c>
+      <c r="V97" t="n">
+        <v>14105</v>
+      </c>
+      <c r="W97" t="s">
+        <v>699</v>
+      </c>
+      <c r="X97" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y97" t="s">
+        <v>706</v>
+      </c>
+      <c r="Z97" t="n">
+        <v>2.567</v>
+      </c>
+      <c r="AA97" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB97" t="n">
+        <v>72</v>
+      </c>
+      <c r="AC97" t="n">
+        <v>38</v>
+      </c>
+      <c r="AD97" t="n">
+        <v>213</v>
+      </c>
+      <c r="AE97" t="n">
+        <v>3318</v>
+      </c>
+      <c r="AF97" t="n">
+        <v>496</v>
+      </c>
+      <c r="AG97" t="n">
+        <v>118</v>
+      </c>
+      <c r="AH97" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="AI97" t="n">
+        <v>87.32</v>
+      </c>
+      <c r="AJ97" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK97" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL97" t="s">
+        <v>306</v>
+      </c>
+      <c r="AM97" t="s">
+        <v>707</v>
+      </c>
+      <c r="AN97" t="n">
+        <v>0.953372189841799</v>
+      </c>
+      <c r="AO97" t="s">
+        <v>695</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>